<commit_message>
All PCB is done, average switch network is created and transfer function tested.
</commit_message>
<xml_diff>
--- a/flyback.xlsx
+++ b/flyback.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\EE_464_hardware_project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="576" yWindow="84" windowWidth="22008" windowHeight="9504"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Sayfa2" sheetId="2" r:id="rId2"/>
     <sheet name="Sayfa3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -249,8 +254,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -399,13 +404,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Ofis Teması">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
   <a:themeElements>
-    <a:clrScheme name="Ofis">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -443,9 +456,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Ofis">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -477,9 +490,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -511,9 +525,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Ofis">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -686,14 +701,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="39.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.109375" customWidth="1"/>
@@ -713,12 +728,12 @@
     <col min="17" max="17" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -730,7 +745,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>36</v>
       </c>
@@ -756,7 +771,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>24</v>
       </c>
@@ -782,7 +797,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -792,7 +807,7 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -802,7 +817,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="7" t="s">
         <v>4</v>
@@ -815,7 +830,7 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>47</v>
       </c>
@@ -827,7 +842,7 @@
       </c>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>40000</v>
       </c>
@@ -839,7 +854,7 @@
       </c>
       <c r="H9" s="4"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
       <c r="B12" s="10" t="s">
         <v>18</v>
@@ -847,7 +862,7 @@
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>41</v>
       </c>
@@ -861,7 +876,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>0.5</v>
       </c>
@@ -875,7 +890,7 @@
         <v>1E-10</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -886,7 +901,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>5</v>
       </c>
@@ -909,7 +924,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <f>(D4/H4)</f>
         <v>75</v>
@@ -939,7 +954,7 @@
         <v>11.116550079742298</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="7" t="s">
         <v>20</v>
@@ -949,7 +964,7 @@
       <c r="E22" s="5"/>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>9</v>
       </c>
@@ -969,7 +984,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <f>G19</f>
         <v>11.116550079742298</v>
@@ -995,14 +1010,14 @@
         <v>7.0149313386750904</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="9"/>
       <c r="B27" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C27" s="9"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>23</v>
       </c>
@@ -1013,7 +1028,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="9">
         <f>(C24*C24)*B14</f>
         <v>1.1667325058559874</v>
@@ -1027,7 +1042,7 @@
         <v>1.2482E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1039,7 +1054,7 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>34</v>
       </c>
@@ -1065,7 +1080,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>1</v>
       </c>
@@ -1092,14 +1107,14 @@
         <v>12.684000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J34" s="17" t="s">
         <v>62</v>
       </c>
       <c r="K34" s="17"/>
       <c r="L34" s="17"/>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J35" s="6">
         <f>(C24/500)*100</f>
         <v>0.96611904270891469</v>
@@ -1109,7 +1124,7 @@
         <v>1.4029862677350182</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="7" t="s">
@@ -1124,7 +1139,7 @@
       <c r="J36" s="6"/>
       <c r="K36" s="6"/>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
         <v>50</v>
       </c>
@@ -1162,7 +1177,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <f>((((A4-D19)*E19)*((A4-D19)*E19))/(2*A9*C19))*1000000</f>
         <v>30.223415648405215</v>
@@ -1212,19 +1227,19 @@
         <v>3.2597636623672845</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D39" s="5">
         <f>SQRT((A38*0.000001)/(B33*0.000000001))</f>
         <v>14.387831532998762</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D40" t="s">
         <v>24</v>
       </c>
       <c r="K40" s="12"/>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>17</v>
       </c>
@@ -1232,7 +1247,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>16</v>
       </c>
@@ -1241,10 +1256,10 @@
       </c>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="10"/>
       <c r="B44" s="11" t="s">
         <v>65</v>
@@ -1252,7 +1267,7 @@
       <c r="C44" s="10"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="s">
         <v>66</v>
       </c>
@@ -1263,7 +1278,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="8">
         <f>F19</f>
         <v>93.4</v>
@@ -1274,7 +1289,7 @@
       </c>
       <c r="C46" s="8"/>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="7"/>
       <c r="B48" s="7" t="s">
         <v>68</v>
@@ -1283,7 +1298,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>73</v>
       </c>
@@ -1292,7 +1307,7 @@
       </c>
       <c r="C49" s="5"/>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
         <f>(C4*(1+B4/C9))*1.3</f>
         <v>49.693548387096776</v>
@@ -1303,13 +1318,13 @@
       </c>
       <c r="C50" s="5"/>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="11" t="s">
         <v>70</v>
       </c>
       <c r="B52" s="11"/>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="11" t="s">
         <v>75</v>
       </c>
@@ -1317,7 +1332,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="9">
         <f>((100*(B19*E19))/(C4*E4*A9))*100000</f>
         <v>9.4412878787878771</v>
@@ -1334,24 +1349,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>